<commit_message>
Changed the output names in XLSX files for Leaf.Tips
</commit_message>
<xml_diff>
--- a/Tests/Validation/Barley/Observations/ABlock99_00_LeafApp.xlsx
+++ b/Tests/Validation/Barley/Observations/ABlock99_00_LeafApp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\ApsimX\Prototypes\Barley\Observations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ApsimX\Tests\Validation\Barley\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF8C3BD-CC04-4A88-B4F4-AE4ACB06F6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="20805"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,13 +141,13 @@
     <t>ABlock99_00SowNovPop400</t>
   </si>
   <si>
-    <t>Barley.Structure.LeafTipsAppeared</t>
+    <t>Barley.Leaf.Tips</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -457,21 +458,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -493,7 +494,7 @@
         <v>2.2749999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -504,7 +505,7 @@
         <v>3.1470000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -515,7 +516,7 @@
         <v>4.2849999999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -526,7 +527,7 @@
         <v>5.1750000000000016</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -537,7 +538,7 @@
         <v>5.9894999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -548,7 +549,7 @@
         <v>7.0600000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -559,7 +560,7 @@
         <v>7.7000000000000011</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -570,7 +571,7 @@
         <v>8.264999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -581,7 +582,7 @@
         <v>9.125</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -592,7 +593,7 @@
         <v>10.034499999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -603,7 +604,7 @@
         <v>10.974999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -614,7 +615,7 @@
         <v>11.620000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -625,7 +626,7 @@
         <v>11.690000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -636,7 +637,7 @@
         <v>11.715000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -647,7 +648,7 @@
         <v>2.3450000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -658,7 +659,7 @@
         <v>3.2144999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -669,7 +670,7 @@
         <v>4.3049999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -680,7 +681,7 @@
         <v>5.1300000000000017</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -691,7 +692,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -702,7 +703,7 @@
         <v>7.0200000000000014</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -713,7 +714,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -724,7 +725,7 @@
         <v>8.3799999999999972</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -735,7 +736,7 @@
         <v>9.1650000000000027</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -746,7 +747,7 @@
         <v>10.154999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -757,7 +758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -768,7 +769,7 @@
         <v>10.844999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -779,7 +780,7 @@
         <v>10.844999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -790,7 +791,7 @@
         <v>10.844999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -801,7 +802,7 @@
         <v>2.3249999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -812,7 +813,7 @@
         <v>3.1800000000000006</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -823,7 +824,7 @@
         <v>4.294999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -834,7 +835,7 @@
         <v>5.004999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -845,7 +846,7 @@
         <v>5.8100000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -856,7 +857,7 @@
         <v>6.9995000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -867,7 +868,7 @@
         <v>7.8149999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -878,7 +879,7 @@
         <v>8.3484999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -889,7 +890,7 @@
         <v>9.1650000000000009</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -900,7 +901,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -911,7 +912,7 @@
         <v>10.655000000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -922,7 +923,7 @@
         <v>10.55</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -933,7 +934,7 @@
         <v>10.55</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -944,7 +945,7 @@
         <v>10.55</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -955,7 +956,7 @@
         <v>2.3149999999999995</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -966,7 +967,7 @@
         <v>3.1300000000000008</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -977,7 +978,7 @@
         <v>4.2344999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -988,7 +989,7 @@
         <v>4.8599999999999994</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>5.6150000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -1010,7 +1011,7 @@
         <v>6.7495000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>7.5649999999999995</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>8.0939999999999994</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -1054,7 +1055,7 @@
         <v>9.8399999999999963</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1065,7 +1066,7 @@
         <v>9.89</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>9.9049999999999994</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -1087,7 +1088,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -1098,7 +1099,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -1109,7 +1110,7 @@
         <v>2.9915000000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -1120,7 +1121,7 @@
         <v>3.2794999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -1131,7 +1132,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>20</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>5.5649999999999995</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -1153,7 +1154,7 @@
         <v>6.28</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -1164,7 +1165,7 @@
         <v>7.3349999999999991</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -1175,7 +1176,7 @@
         <v>8.4550000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -1186,7 +1187,7 @@
         <v>9.6795000000000009</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>20</v>
       </c>
@@ -1197,7 +1198,7 @@
         <v>9.9344999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>20</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>9.9495000000000005</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>3.0245000000000011</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>25</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>3.3699999999999988</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>25</v>
       </c>
@@ -1241,7 +1242,7 @@
         <v>4.589999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>25</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>5.5649999999999995</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>25</v>
       </c>
@@ -1263,7 +1264,7 @@
         <v>6.2750000000000012</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>25</v>
       </c>
@@ -1274,7 +1275,7 @@
         <v>7.4599999999999991</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>25</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>8.5299999999999994</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -1296,7 +1297,7 @@
         <v>9.8199999999999985</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>25</v>
       </c>
@@ -1307,7 +1308,7 @@
         <v>9.84</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>25</v>
       </c>
@@ -1318,7 +1319,7 @@
         <v>9.84</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -1329,7 +1330,7 @@
         <v>2.959000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>26</v>
       </c>
@@ -1340,7 +1341,7 @@
         <v>3.2894999999999994</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>26</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>4.5249999999999995</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>26</v>
       </c>
@@ -1362,7 +1363,7 @@
         <v>5.4349999999999996</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>6.14</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>26</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>7.2245000000000008</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>26</v>
       </c>
@@ -1395,7 +1396,7 @@
         <v>8.370000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -1406,7 +1407,7 @@
         <v>9.5595000000000017</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>26</v>
       </c>
@@ -1417,7 +1418,7 @@
         <v>9.6199999999999992</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -1428,7 +1429,7 @@
         <v>9.6199999999999992</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>27</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>2.9625000000000008</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>27</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>3.2049999999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>27</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>4.3149999999999995</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>27</v>
       </c>
@@ -1472,7 +1473,7 @@
         <v>5.1644999999999994</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>27</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>5.8039999999999994</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>27</v>
       </c>
@@ -1494,7 +1495,7 @@
         <v>6.9450000000000003</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>27</v>
       </c>
@@ -1505,7 +1506,7 @@
         <v>8.2249999999999996</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>27</v>
       </c>
@@ -1516,7 +1517,7 @@
         <v>9.2149999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>27</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>8.9349999999999987</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>27</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>8.9349999999999987</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>28</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>4.05</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>28</v>
       </c>
@@ -1560,7 +1561,7 @@
         <v>5.71</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>28</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>7.205000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>28</v>
       </c>
@@ -1582,7 +1583,7 @@
         <v>9.6399999999999988</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>28</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>9.8049999999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>28</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>9.8049999999999997</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>35</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>4.2359999999999989</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>35</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>5.7439999999999998</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>35</v>
       </c>
@@ -1637,7 +1638,7 @@
         <v>7.128000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>35</v>
       </c>
@@ -1648,7 +1649,7 @@
         <v>8.8160000000000007</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>35</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>8.7959999999999994</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>35</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>8.7959999999999994</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>36</v>
       </c>
@@ -1681,7 +1682,7 @@
         <v>4.1899999999999995</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>36</v>
       </c>
@@ -1692,7 +1693,7 @@
         <v>5.7249999999999996</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>36</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>7.01</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>36</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>36</v>
       </c>
@@ -1725,7 +1726,7 @@
         <v>8.9599999999999991</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -1736,7 +1737,7 @@
         <v>8.9599999999999991</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>37</v>
       </c>
@@ -1747,7 +1748,7 @@
         <v>4.1933333333333325</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>37</v>
       </c>
@@ -1758,7 +1759,7 @@
         <v>5.753333333333333</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>37</v>
       </c>
@@ -1769,7 +1770,7 @@
         <v>7.1399999999999988</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>37</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>37</v>
       </c>
@@ -1791,7 +1792,7 @@
         <v>8.9333333333333336</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>37</v>
       </c>

</xml_diff>